<commit_message>
fixes to grid search
</commit_message>
<xml_diff>
--- a/Grid_search_0.xlsx
+++ b/Grid_search_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -546,23 +546,23 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[0.09090909090909091, 0.3, 0.3, 0.2, 0.2, 0.3, 0.2, 0.3, 0.3, 0.3, 0.3, 0.1, 0.3, 0.3, 0.3, 0.2, 0.4, 0.3, 0.5, 0.3, 0.1, 0.4, 0.3, 0.2, 0.3, 0.2, 0.1, 0.4, 0.2, 0.3, 0.4, 0.3, 0.2, 0.2, 0.2, 0.4, 0.5, 0.1, 0.2, 0.2, 0.0, 0.1, 0.1, 0.1, 0.0, 0.3, 0.3, 0.4, 0.2, 0.2, 0.6, 0.3, 0.1, 0.2, 0.3, 0.4, 0.3, 0.3, 0.4, 0.4, 0.4, 0.2, 0.3, 0.2, 0.3, 0.1, 0.3, 0.3, 0.1, 0.5, 0.0, 0.3, 0.2, 0.1, 0.0, 0.4, 0.4, 0.4, 0.1, 0.1, 0.1, 0.1, 0.2, 0.0, 0.4, 0.2, 0.2, 0.3, 0.1, 0.5, 0.2, 0.3, 0.2, 0.1, 0.1, 0.1, 0.1, 0.3, 0.2]</t>
+          <t>[0.45454545454545453, 0.2, 0.1, 0.4, 0.2, 0.3, 0.4, 0.1, 0.2, 0.3, 0.1, 0.2, 0.4, 0.2, 0.0, 0.1, 0.2, 0.3, 0.4, 0.5, 0.4, 0.0, 0.4, 0.3, 0.4, 0.6, 0.4, 0.3, 0.3, 0.0, 0.2, 0.1, 0.2, 0.1, 0.3, 0.2, 0.2, 0.0, 0.1, 0.3, 0.2, 0.0, 0.4, 0.2, 0.1, 0.5, 0.2, 0.2, 0.3, 0.5, 0.2, 0.4, 0.1, 0.1, 0.1, 0.1, 0.2, 0.1, 0.1, 0.2, 0.2, 0.1, 0.0, 0.4, 0.3, 0.3, 0.3, 0.1, 0.2, 0.2, 0.4, 0.4, 0.5, 0.2, 0.4, 0.2, 0.2, 0.3, 0.1, 0.3, 0.3, 0.2, 0.1, 0.3, 0.4, 0.3, 0.2, 0.3, 0.0, 0.2, 0.3, 0.2, 0.3, 0.3, 0.2, 0.5, 0.3, 0.2, 0.3, 0.4, 0.3, 0.2, 0.2, 0.1, 0.4, 0.1, 0.0, 0.1, 0.3, 0.2, 0.4, 0.2, 0.0, 0.4, 0.2, 0.2, 0.0, 0.3, 0.4, 0.0, 0.2, 0.2, 0.3, 0.4, 0.2, 0.2, 0.5, 0.4, 0.3, 0.0, 0.3, 0.3, 0.2, 0.4, 0.2, 0.2, 0.5, 0.2, 0.0, 0.3, 0.4, 0.2, 0.1, 0.3, 0.4, 0.1, 0.3, 0.1, 0.3, 0.4, 0.4, 0.2, 0.0, 0.2, 0.3, 0.3, 0.2, 0.6, 0.1, 0.3, 0.3, 0.4, 0.3, 0.3, 0.8, 0.2, 0.4, 0.1, 0.4, 0.2, 0.2, 0.1, 0.2, 0.3, 0.2, 0.3, 0.5, 0.1, 0.6, 0.1, 0.3, 0.1, 0.8, 0.3, 0.4, 0.2, 0.2, 0.4, 0.3, 0.3, 0.4, 0.5, 0.2, 0.2, 0.6, 0.4, 0.4, 0.3, 0.2, 0.0, 0.3, 0.3, 0.4, 0.4, 0.0, 0.4, 0.2, 0.1, 0.2, 0.2, 0.2, 0.2, 0.5, 0.2, 0.5, 0.1, 0.5, 0.5, 0.2, 0.4, 0.4, 0.2, 0.2, 0.2, 0.0, 0.4, 0.3, 0.3, 0.0, 0.2, 0.6, 0.0, 0.3, 0.1, 0.1, 0.1, 0.1, 0.2, 0.2, 0.3, 0.4, 0.2, 0.1, 0.3, 0.2, 0.1, 0.2, 0.4, 0.5, 0.1, 0.1, 0.3, 0.5, 0.1, 0.3, 0.3, 0.1, 0.2, 0.1, 0.2, 0.2, 0.2, 0.0, 0.3, 0.2, 0.0, 0.5, 0.3, 0.2, 0.1, 0.1, 0.0, 0.4, 0.5, 0.4, 0.2, 0.3, 0.0, 0.0, 0.2, 0.1, 0.3, 0.1, 0.4, 0.3, 0.1, 0.0, 0.6, 0.3, 0.3, 0.5, 0.2, 0.2, 0.4, 0.2, 0.2, 0.3, 0.3, 0.2, 0.1, 0.2, 0.3, 0.2, 0.3, 0.1, 0.3, 0.2, 0.2, 0.1, 0.2, 0.1, 0.2, 0.5, 0.1, 0.1, 0.5, 0.3, 0.3, 0.5, 0.3, 0.2, 0.1, 0.1, 0.1, 0.4, 0.3, 0.1, 0.4, 0.5, 0.0, 0.3, 0.2, 0.1, 0.7, 0.1, 0.2, 0.3, 0.3, 0.4, 0.3, 0.3, 0.3, 0.2, 0.2, 0.2, 0.2, 0.0, 0.2, 0.4, 0.3, 0.2, 0.3, 0.1, 0.1, 0.5, 0.3, 0.4, 0.5, 0.3, 0.3, 0.3, 0.2, 0.4, 0.1, 0.2, 0.2, 0.2, 0.3, 0.2, 0.2, 0.2, 0.3, 0.3, 0.1, 0.4, 0.4, 0.1, 0.1, 0.5, 0.2, 0.3, 0.2, 0.2, 0.2, 0.1, 0.1, 0.5, 0.1, 0.1, 0.2, 0.2, 0.1, 0.1, 0.2, 0.3, 0.3, 0.1, 0.3, 0.2, 0.3, 0.1, 0.2, 0.3, 0.3, 0.1, 0.1, 0.1, 0.2, 0.2, 0.1, 0.2, 0.2, 0.1, 0.4, 0.0, 0.1, 0.0, 0.2, 0.1, 0.4, 0.1, 0.1, 0.2, 0.1, 0.5, 0.4, 0.1, 0.3, 0.3, 0.2, 0.4, 0.1, 0.3, 0.3, 0.2, 0.1, 0.4, 0.3, 0.0, 0.5, 0.3, 0.1, 0.1, 0.2, 0.1, 0.2, 0.1, 0.2, 0.2, 0.2, 0.2, 0.2, 0.2, 0.3, 0.1, 0.0, 0.2, 0.3, 0.2, 0.2, 0.2, 0.1, 0.4, 0.1, 0.4, 0.3, 0.5, 0.1, 0.5, 0.1, 0.2, 0.2, 0.3, 0.2, 0.2, 0.2, 0.3, 0.4, 0.2, 0.2, 0.3, 0.1, 0.2, 0.3, 0.5, 0.3, 0.1, 0.3, 0.2, 0.5, 0.3, 0.2, 0.3, 0.3, 0.1, 0.4, 0.2, 0.2, 0.1]</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>0.21</v>
+        <v>0.2600000000000001</v>
       </c>
       <c r="N2" t="n">
-        <v>0.33</v>
+        <v>0.3799999999999999</v>
       </c>
       <c r="O2" t="n">
-        <v>600</v>
+        <v>1920</v>
       </c>
       <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -596,269 +596,19 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[0.18181818181818182, 0.3, 0.1, 0.2, 0.1, 0.3, 0.3, 0.0, 0.4, 0.2, 0.2, 0.2, 0.1, 0.2, 0.2, 0.2, 0.2, 0.3, 0.1, 0.2, 0.0, 0.2, 0.2, 0.0, 0.4, 0.2, 0.4, 0.2, 0.3, 0.2, 0.2, 0.2, 0.2, 0.2, 0.1, 0.3, 0.3, 0.2, 0.3, 0.1, 0.3, 0.4, 0.3, 0.3, 0.4, 0.3, 0.3, 0.2, 0.1, 0.3, 0.3, 0.2, 0.0, 0.2, 0.3, 0.3, 0.1, 0.4, 0.4, 0.4, 0.1, 0.0, 0.3, 0.0, 0.7, 0.3, 0.4, 0.2, 0.1, 0.5, 0.0, 0.3, 0.2, 0.1, 0.1, 0.3, 0.4, 0.2, 0.3, 0.3, 0.1, 0.0, 0.3, 0.6, 0.0, 0.1, 0.1, 0.1, 0.4, 0.4, 0.2, 0.0, 0.2, 0.2, 0.4, 0.3, 0.3, 0.4, 0.6]</t>
+          <t>[0.36363636363636365, 0.4, 0.3, 0.3, 0.3, 0.6, 0.2, 0.2, 0.0, 0.5, 0.3, 0.2, 0.1, 0.2, 0.2, 0.3, 0.4, 0.2, 0.5, 0.1, 0.4, 0.3, 0.1, 0.5, 0.2, 0.4, 0.2, 0.4, 0.4, 0.4, 0.1, 0.3, 0.1, 0.2, 0.2, 0.3, 0.4, 0.3, 0.0, 0.1, 0.2, 0.2, 0.3, 0.1, 0.2, 0.4, 0.1, 0.3, 0.4, 0.1, 0.5, 0.2, 0.2, 0.0, 0.3, 0.2, 0.2, 0.2, 0.3, 0.1, 0.3, 0.3, 0.3, 0.3, 0.4, 0.3, 0.1, 0.1, 0.3, 0.1, 0.5, 0.0, 0.3, 0.2, 0.6, 0.3, 0.4, 0.3, 0.5, 0.2, 0.2, 0.4, 0.5, 0.5, 0.1, 0.2, 0.3, 0.0, 0.1, 0.0, 0.1, 0.2, 0.2, 0.1, 0.6, 0.2, 0.5, 0.4, 0.2, 0.2, 0.4, 0.6, 0.1, 0.2, 0.2, 0.3, 0.4, 0.4, 0.2, 0.3, 0.7, 0.1, 0.2, 0.4, 0.4, 0.3, 0.4, 0.3, 0.2, 0.3, 0.4, 0.2, 0.4, 0.2, 0.3, 0.1, 0.2, 0.0, 0.3, 0.5, 0.4, 0.3, 0.3, 0.4, 0.4, 0.1, 0.2, 0.2, 0.2, 0.5, 0.5, 0.5, 0.3, 0.5, 0.4, 0.1, 0.2, 0.4, 0.3, 0.4, 0.1, 0.4, 0.3, 0.2, 0.2, 0.3, 0.3, 0.2, 0.3, 0.6, 0.3, 0.2, 0.3, 0.2, 0.2, 0.2, 0.1, 0.3, 0.5, 0.4, 0.2, 0.3, 0.4, 0.2, 0.3, 0.4, 0.4, 0.4, 0.0, 0.2, 0.2, 0.2, 0.3, 0.3, 0.4, 0.2, 0.5, 0.2, 0.2, 0.1, 0.1, 0.0, 0.3, 0.1, 0.4, 0.3, 0.5, 0.2, 0.1, 0.4, 0.4, 0.2, 0.3, 0.3, 0.1, 0.3, 0.1, 0.3, 0.4, 0.3, 0.5, 0.2, 0.5, 0.7, 0.1, 0.1, 0.1, 0.4, 0.2, 0.4, 0.4, 0.2, 0.3, 0.0, 0.3, 0.2, 0.4, 0.3, 0.3, 0.5, 0.2, 0.5, 0.3, 0.3, 0.2, 0.3, 0.4, 0.1, 0.5, 0.2, 0.3, 0.4, 0.2, 0.1, 0.0, 0.3, 0.2, 0.4, 0.4, 0.2, 0.2, 0.4, 0.4, 0.5, 0.3, 0.3, 0.2, 0.3, 0.3, 0.2, 0.3, 0.2, 0.4, 0.2, 0.3, 0.3, 0.4, 0.1, 0.2, 0.1, 0.1, 0.2, 0.5, 0.3, 0.1, 0.1, 0.3, 0.2, 0.1, 0.1, 0.1, 0.2, 0.3, 0.2, 0.2, 0.2, 0.2, 0.5, 0.5, 0.1, 0.1, 0.2, 0.5, 0.3, 0.3, 0.2, 0.4, 0.4, 0.1, 0.0, 0.1, 0.5, 0.2, 0.3, 0.1, 0.4, 0.0, 0.0, 0.3, 0.1, 0.1, 0.2, 0.1, 0.2, 0.3, 0.1, 0.2, 0.4, 0.4, 0.1, 0.2, 0.1, 0.7, 0.0, 0.3, 0.4, 0.1, 0.1, 0.4, 0.2, 0.1, 0.3, 0.3, 0.3, 0.2, 0.2, 0.3, 0.4, 0.4, 0.2, 0.3, 0.2, 0.2, 0.1, 0.3, 0.2, 0.4, 0.4, 0.1, 0.4, 0.1, 0.4, 0.2, 0.1, 0.1, 0.3, 0.3, 0.2, 0.4, 0.2, 0.2, 0.5, 0.1, 0.2, 0.2, 0.1, 0.1, 0.4, 0.4, 0.5, 0.0, 0.3, 0.2, 0.3, 0.2, 0.2, 0.4, 0.1, 0.3, 0.4, 0.3, 0.3, 0.2, 0.1, 0.2, 0.2, 0.3, 0.2, 0.4, 0.1, 0.3, 0.2, 0.4, 0.4, 0.3, 0.2, 0.1, 0.5, 0.2, 0.1, 0.3, 0.4, 0.1, 0.1, 0.2, 0.2, 0.2, 0.2, 0.1, 0.4, 0.3, 0.0, 0.1, 0.5, 0.2, 0.3, 0.5, 0.3, 0.2, 0.2, 0.2, 0.2, 0.2, 0.2, 0.3, 0.2, 0.3, 0.6, 0.2, 0.2, 0.1, 0.6, 0.1, 0.3, 0.2, 0.4, 0.5, 0.4, 0.3, 0.4, 0.2, 0.4, 0.2, 0.2, 0.4, 0.4, 0.2, 0.3, 0.2, 0.2, 0.4, 0.3, 0.2, 0.7, 0.4, 0.4, 0.1, 0.3, 0.2, 0.3, 0.2, 0.2, 0.2, 0.6, 0.2, 0.1, 0.1, 0.2, 0.2, 0.2, 0.1, 0.5, 0.1, 0.2, 0.4, 0.3, 0.3, 0.3, 0.2, 0.4, 0.6, 0.1, 0.3, 0.1, 0.1, 0.1, 0.2, 0.2, 0.3, 0.4, 0.4, 0.3, 0.1, 0.2, 0.4, 0.0, 0.1, 0.3, 0.0]</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="N3" t="n">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
       <c r="O3" t="n">
-        <v>670</v>
+        <v>840</v>
       </c>
       <c r="P3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>32</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="I4" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>[0.36363636363636365, 0.3, 0.2, 0.3, 0.1, 0.1, 0.4, 0.5, 0.1, 0.1, 0.2, 0.2, 0.2, 0.2, 0.1, 0.0, 0.3, 0.2, 0.3, 0.3, 0.3, 0.3, 0.2, 0.2, 0.1, 0.2, 0.3, 0.1, 0.4, 0.3, 0.1, 0.5, 0.0, 0.3, 0.1, 0.1, 0.3, 0.6, 0.2, 0.4, 0.3, 0.3, 0.2, 0.1, 0.3, 0.3, 0.5, 0.1, 0.1, 0.4, 0.7, 0.2, 0.2, 0.0, 0.3, 0.4, 0.5, 0.2, 0.3, 0.3, 0.2, 0.3, 0.3, 0.3, 0.5, 0.2, 0.1, 0.2, 0.3, 0.3, 0.2, 0.5, 0.5, 0.4, 0.1, 0.4, 0.5, 0.3, 0.2, 0.1, 0.4, 0.1, 0.4, 0.3, 0.0, 0.1, 0.2, 0.2, 0.5, 0.0, 0.1, 0.3, 0.0, 0.2, 0.2, 0.4, 0.1, 0.3, 0.3]</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="O4" t="n">
-        <v>780</v>
-      </c>
-      <c r="P4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>32</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
-        <v>50</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>[0.18181818181818182, 0.1, 0.1, 0.3, 0.4, 0.1, 0.2, 0.4, 0.4, 0.2, 0.2, 0.3, 0.2, 0.3, 0.2, 0.3, 0.4, 0.3, 0.1, 0.1, 0.2, 0.3, 0.1, 0.3, 0.3, 0.3, 0.2, 0.1, 0.6, 0.3, 0.2, 0.1, 0.2, 0.2, 0.2, 0.0, 0.1, 0.3, 0.2, 0.1, 0.2, 0.2, 0.2, 0.0, 0.2, 0.3, 0.2, 0.4, 0.1, 0.1, 0.3, 0.3, 0.5, 0.3, 0.2, 0.1, 0.2, 0.6, 0.1, 0.3, 0.5, 0.3, 0.5, 0.2, 0.3, 0.5, 0.3, 0.2, 0.3, 0.1, 0.3, 0.1, 0.3, 0.3, 0.2, 0.2, 0.2, 0.3, 0.3, 0.3, 0.3, 0.2, 0.2, 0.5, 0.1, 0.3, 0.2, 0.3, 0.7, 0.5, 0.2, 0.3, 0.3, 0.3, 0.3, 0.3, 0.2, 0.2, 0.3]</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="O5" t="n">
-        <v>670</v>
-      </c>
-      <c r="P5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>32</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="I6" t="n">
-        <v>5000</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>50</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>[0.09090909090909091, 0.1, 0.3, 0.3, 0.2, 0.3, 0.2, 0.1, 0.1, 0.1, 0.4, 0.2, 0.1, 0.4, 0.3, 0.1, 0.4, 0.5, 0.2, 0.2, 0.1, 0.2, 0.2, 0.0, 0.3, 0.4, 0.2, 0.2, 0.2, 0.5, 0.4, 0.3, 0.2, 0.3, 0.1, 0.4, 0.4, 0.4, 0.2, 0.3, 0.3, 0.0, 0.2, 0.0, 0.4, 0.6, 0.1, 0.4, 0.3, 0.0, 0.3, 0.3, 0.2, 0.4, 0.3, 0.2, 0.0, 0.2, 0.3, 0.3, 0.4, 0.1, 0.3, 0.4, 0.3, 0.3, 0.2, 0.2, 0.2, 0.4, 0.3, 0.3, 0.1, 0.4, 0.3, 0.2, 0.3, 0.1, 0.2, 0.4, 0.1, 0.1, 0.2, 0.1, 0.1, 0.4, 0.2, 0.1, 0.4, 0.4, 0.3, 0.2, 0.4, 0.2, 0.1, 0.3, 0.4, 0.4, 0.4]</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>0.3099999999999999</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="O6" t="n">
-        <v>390</v>
-      </c>
-      <c r="P6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>32</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>10</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>[0.45454545454545453, 0.3, 0.3, 0.0, 0.2, 0.1, 0.3, 0.2, 0.1, 0.3, 0.3, 0.2, 0.2, 0.3, 0.4, 0.4, 0.4, 0.1, 0.1, 0.1, 0.1, 0.2, 0.2, 0.0, 0.4, 0.2, 0.5, 0.5, 0.1, 0.3, 0.1, 0.2, 0.2, 0.0, 0.2, 0.3, 0.1, 0.2, 0.1, 0.1, 0.3, 0.3, 0.3, 0.2, 0.4, 0.3, 0.3, 0.2, 0.4, 0.3, 0.2, 0.1, 0.2, 0.2, 0.3, 0.2, 0.1, 0.2, 0.4, 0.2, 0.1, 0.3, 0.2, 0.1, 0.2, 0.0, 0.1, 0.6, 0.1, 0.2, 0.4, 0.3, 0.4, 0.1, 0.4, 0.2, 0.1, 0.4, 0.3, 0.2, 0.3, 0.3, 0.1, 0.4, 0.3, 0.6, 0.2, 0.3, 0.2, 0.3, 0.3, 0.2, 0.5, 0.3, 0.0, 0.3, 0.2, 0.2, 0.5]</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="O7" t="n">
-        <v>930</v>
-      </c>
-      <c r="P7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>32</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
-        <v>50</v>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>[0.09090909090909091, 0.0, 0.1, 0.0, 0.1, 0.2, 0.4, 0.2, 0.1, 0.2, 0.1, 0.3, 0.3, 0.1, 0.0, 0.4, 0.2, 0.2, 0.1, 0.4, 0.1, 0.4, 0.0, 0.1, 0.2, 0.3, 0.6, 0.4, 0.3, 0.0, 0.3, 0.1, 0.2, 0.3, 0.1, 0.1, 0.0, 0.2, 0.3, 0.4, 0.0, 0.3, 0.3, 0.5, 0.4, 0.7, 0.0, 0.2, 0.3, 0.1, 0.1, 0.4, 0.4, 0.1, 0.2, 0.2, 0.4, 0.6, 0.3, 0.3, 0.3, 0.2, 0.3, 0.0, 0.1, 0.1, 0.3, 0.2, 0.4, 0.2, 0.3, 0.1, 0.4, 0.3, 0.1, 0.5, 0.3, 0.2, 0.2, 0.2, 0.4, 0.3, 0.5, 0.3, 0.3, 0.5, 0.0, 0.1, 0.2, 0.3, 0.6, 0.1, 0.6, 0.3, 0.2, 0.3, 0.3, 0.5, 0.5]</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="O8" t="n">
-        <v>990</v>
-      </c>
-      <c r="P8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>